<commit_message>
add logging of arguments/command to dfr_evaluate. updated test_results spreadsheet
</commit_message>
<xml_diff>
--- a/evidence/test_results.xlsx
+++ b/evidence/test_results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\deep_learning_project\DPBIA_deep_feature_reweighting\evidence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C28751-DD63-4FD7-B2BA-D68209E32C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B745494-C468-461A-9767-9B2C606FFE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19875" yWindow="0" windowWidth="37725" windowHeight="23400" xr2:uid="{327FB3C0-889A-4FD5-9955-D7EA4D55226C}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="23400" activeTab="2" xr2:uid="{327FB3C0-889A-4FD5-9955-D7EA4D55226C}"/>
   </bookViews>
   <sheets>
-    <sheet name="train_classifier" sheetId="1" r:id="rId1"/>
-    <sheet name="dfr" sheetId="2" r:id="rId2"/>
+    <sheet name="train_classifier WB" sheetId="1" r:id="rId1"/>
+    <sheet name="dfr WB" sheetId="2" r:id="rId2"/>
+    <sheet name="train_classifier CelebA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="207">
   <si>
     <t>--data_dir=../data/waterbird_complete95_forest2water2/  --output_dir=RSLTS_DFR  --ckpt_path=RSLTS_TC_2024-03-21_100243/final_checkpoint.pt --tune_class_weights_dfr_train</t>
   </si>
@@ -894,6 +895,140 @@
   </si>
   <si>
     <t>Val</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C:\deep_learning_project\DPBIA_deep_feature_reweighting\train_classifier.py </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>--output_dir=RSLTS_TC --pretrained_model --num_epochs=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF2AACB8"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">100 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>--weight_decay=1e-3 --batch_size=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF2AACB8"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">32 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>--init_lr=1e-3 --eval_freq=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF2AACB8"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>--data_dir=../data/waterbird_complete95_forest2water2/ --test_wb_dir=../data/waterbird_complete95_forest2water2/ --augment_data --seed=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF2AACB8"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>16</t>
+    </r>
+  </si>
+  <si>
+    <t>Epoch 99     Loss: 0.00018200380145572126</t>
+  </si>
+  <si>
+    <t>{'accuracy_0_0': 0.9968957871396896, 'accuracy_0_1': 0.8518847006651885, 'accuracy_1_0': 0.7383177570093458, 'accuracy_1_1': 0.9657320872274143, 'mean_accuracy': 0.9083534691059717, 'worst_accuracy': 0.7383177570093458}</t>
+  </si>
+  <si>
+    <t>{'accuracy_0_0': 0.9957173447537473, 'accuracy_0_1': 0.8304721030042919, 'accuracy_1_0': 0.706766917293233, 'accuracy_1_1': 0.9624060150375939, 'mean_accuracy': 0.8957464553794829, 'worst_accuracy': 0.706766917293233}</t>
+  </si>
+  <si>
+    <t>Preparing directory CELEBA_RSLTS_TC_2024-04-05_130546</t>
+  </si>
+  <si>
+    <t>Training Data (total 162770)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 0 (y=0, p=0): n = 71629</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 1 (y=0, p=1): n = 66874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 2 (y=1, p=0): n = 22880</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 3 (y=1, p=1): n = 1387</t>
+  </si>
+  <si>
+    <t>Test Data (total 19962)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 0 (y=0, p=0): n = 9767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 1 (y=0, p=1): n = 7535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 2 (y=1, p=0): n = 2480</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 3 (y=1, p=1): n = 180</t>
+  </si>
+  <si>
+    <t>Validation Data (total 19867)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 0 (y=0, p=0): n = 8535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 1 (y=0, p=1): n = 8276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 2 (y=1, p=0): n = 2874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Group 3 (y=1, p=1): n = 182</t>
   </si>
 </sst>
 </file>
@@ -1343,14 +1478,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BF2C77-194D-4C74-8EF8-245AE7739130}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1626,7 +1762,7 @@
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="6"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="8" t="s">
         <v>152</v>
       </c>
@@ -1639,7 +1775,9 @@
       <c r="E25" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="8" t="s">
+        <v>187</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
@@ -1652,7 +1790,7 @@
         <v>42</v>
       </c>
       <c r="C26" s="8" t="str">
-        <f t="shared" ref="C26:E26" si="0">RIGHT(C25,LEN(C25)-FIND("seed=",C25)-4)</f>
+        <f t="shared" ref="C26:F26" si="0">RIGHT(C25,LEN(C25)-FIND("seed=",C25)-4)</f>
         <v>7</v>
       </c>
       <c r="D26" s="8" t="str">
@@ -1663,7 +1801,10 @@
         <f t="shared" si="0"/>
         <v>747</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
@@ -1681,7 +1822,9 @@
       <c r="E27" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="8" t="s">
+        <v>188</v>
+      </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
@@ -1699,7 +1842,9 @@
       <c r="E28" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="F28" s="6"/>
+      <c r="F28" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
@@ -1717,7 +1862,9 @@
       <c r="E29" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
@@ -1735,7 +1882,9 @@
       <c r="E30" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="8" t="s">
+        <v>148</v>
+      </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
     </row>
@@ -1753,7 +1902,9 @@
       <c r="E31" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="8" t="s">
+        <v>189</v>
+      </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
     </row>
@@ -1771,7 +1922,9 @@
       <c r="E32" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="F32" s="6"/>
+      <c r="F32" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
     </row>
@@ -1789,7 +1942,9 @@
       <c r="E33" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="F33" s="6"/>
+      <c r="F33" s="8" t="s">
+        <v>190</v>
+      </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
@@ -1829,7 +1984,10 @@
         <f t="shared" si="1"/>
         <v>0.90852606144287196</v>
       </c>
-      <c r="F35" s="6"/>
+      <c r="F35" s="10">
+        <f t="shared" ref="F35" si="2">_xlfn.NUMBERVALUE(MID(F31,LEN(F31)-56,18))</f>
+        <v>0.90835346910597103</v>
+      </c>
       <c r="G35" s="11">
         <f>AVERAGE(B35:E35)</f>
         <v>0.91141698308595054</v>
@@ -1848,18 +2006,21 @@
         <v>0.71183800623052895</v>
       </c>
       <c r="C36" s="10">
-        <f t="shared" ref="C36:E36" si="2">_xlfn.NUMBERVALUE(MID(C31,LEN(C31)-19,18))</f>
+        <f t="shared" ref="C36:E36" si="3">_xlfn.NUMBERVALUE(MID(C31,LEN(C31)-19,18))</f>
         <v>0.78816199376947005</v>
       </c>
       <c r="D36" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.66822429906542002</v>
       </c>
       <c r="E36" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.741433021806853</v>
       </c>
-      <c r="F36" s="6"/>
+      <c r="F36" s="10">
+        <f t="shared" ref="F36" si="4">_xlfn.NUMBERVALUE(MID(F31,LEN(F31)-19,18))</f>
+        <v>0.73831775700934499</v>
+      </c>
       <c r="G36" s="11">
         <f>AVERAGE(B36:E36)</f>
         <v>0.72741433021806801</v>
@@ -1877,7 +2038,7 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="6"/>
+      <c r="F37" s="10"/>
       <c r="G37" s="11"/>
       <c r="H37" s="4"/>
     </row>
@@ -1890,18 +2051,21 @@
         <v>0.90575479566305195</v>
       </c>
       <c r="C38" s="10">
-        <f t="shared" ref="C38:E38" si="3">_xlfn.NUMBERVALUE(MID(C33,LEN(C33)-56,18))</f>
+        <f t="shared" ref="C38:E38" si="5">_xlfn.NUMBERVALUE(MID(C33,LEN(C33)-56,18))</f>
         <v>0.90825688073394495</v>
       </c>
       <c r="D38" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.90825688073394495</v>
       </c>
       <c r="E38" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.89658048373644705</v>
       </c>
-      <c r="F38" s="6"/>
+      <c r="F38" s="10">
+        <f t="shared" ref="F38" si="6">_xlfn.NUMBERVALUE(MID(F33,LEN(F33)-56,18))</f>
+        <v>0.89574645537948205</v>
+      </c>
       <c r="G38" s="11">
         <f>AVERAGE(B38:E38)</f>
         <v>0.90471226021684725</v>
@@ -1920,18 +2084,21 @@
         <v>0.721804511278195</v>
       </c>
       <c r="C39" s="10">
-        <f t="shared" ref="C39:E39" si="4">_xlfn.NUMBERVALUE(MID(C33,LEN(C33)-19,18))</f>
+        <f t="shared" ref="C39:E39" si="7">_xlfn.NUMBERVALUE(MID(C33,LEN(C33)-19,18))</f>
         <v>0.80451127819548796</v>
       </c>
       <c r="D39" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.66165413533834505</v>
       </c>
       <c r="E39" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.69924812030075101</v>
       </c>
-      <c r="F39" s="6"/>
+      <c r="F39" s="10">
+        <f>_xlfn.NUMBERVALUE(MID(F33,LEN(F33)-18,17))</f>
+        <v>0.70676691729323005</v>
+      </c>
       <c r="G39" s="11">
         <f>AVERAGE(B39:E39)</f>
         <v>0.72180451127819478</v>
@@ -1943,6 +2110,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3153,4 +3321,129 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915E905E-2A03-4723-878F-B49E2B2557DF}">
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>202599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>162770</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>202599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>19962</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>202599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>19867</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Results of DFR into spreadsheet
</commit_message>
<xml_diff>
--- a/evidence/test_results.xlsx
+++ b/evidence/test_results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\deep_learning_project\DPBIA_deep_feature_reweighting\evidence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B745494-C468-461A-9767-9B2C606FFE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F72348-F73D-4F65-B280-91169C5953E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="23400" activeTab="2" xr2:uid="{327FB3C0-889A-4FD5-9955-D7EA4D55226C}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="23400" activeTab="3" xr2:uid="{327FB3C0-889A-4FD5-9955-D7EA4D55226C}"/>
   </bookViews>
   <sheets>
     <sheet name="train_classifier WB" sheetId="1" r:id="rId1"/>
     <sheet name="dfr WB" sheetId="2" r:id="rId2"/>
     <sheet name="train_classifier CelebA" sheetId="3" r:id="rId3"/>
+    <sheet name="dfr CelebA" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +38,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1049BCA2-D16F-4A49-86F1-791FBB17D5A7}</author>
+  </authors>
+  <commentList>
+    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{1049BCA2-D16F-4A49-86F1-791FBB17D5A7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Interupted run - ran epochs 0-11 then 0-38 (which is 51 rather than intended 50)</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="322">
   <si>
     <t>--data_dir=../data/waterbird_complete95_forest2water2/  --output_dir=RSLTS_DFR  --ckpt_path=RSLTS_TC_2024-03-21_100243/final_checkpoint.pt --tune_class_weights_dfr_train</t>
   </si>
@@ -1030,15 +1049,371 @@
   <si>
     <t xml:space="preserve">    Group 3 (y=1, p=1): n = 182</t>
   </si>
+  <si>
+    <t>Epoch 38     Loss: 0.006819494534283876</t>
+  </si>
+  <si>
+    <t>{'accuracy_0_0': 0.9976825028968713, 'accuracy_0_1': 0.9995813021503125, 'accuracy_1_0': 0.9938811188811189, 'accuracy_1_1': 0.9790915645277577, 'mean_accuracy': 0.9977698593106837, 'worst_accuracy': 0.9790915645277577}</t>
+  </si>
+  <si>
+    <t>{'accuracy_0_0': 0.9600696221971946, 'accuracy_0_1': 0.993364299933643, 'accuracy_1_0': 0.8407258064516129, 'accuracy_1_1': 0.42777777777777776, 'mean_accuracy': 0.9530107203687005, 'worst_accuracy': 0.42777777777777776}</t>
+  </si>
+  <si>
+    <t>{'accuracy_0_0': 0.9516110134739308, 'accuracy_0_1': 0.9942000966650556, 'accuracy_1_0': 0.8583855254001391, 'accuracy_1_1': 0.37362637362637363, 'mean_accuracy': 0.9505712991392762, 'worst_accuracy': 0.37362637362637363}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C:\deep_learning_project\DPBIA_deep_feature_reweighting\train_classifier.py </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>--output_dir=CELEBA_RSLTS_TC --pretrained_model --num_epochs=50 --weight_decay=1e-4 --batch_size=64 --init_lr=1e-3 --eval_freq=1 --data_dir=../data/celebA/ --test_wb_dir=../data/celebA/ --augment_data --seed=16</t>
+    </r>
+  </si>
+  <si>
+    <t>--data_dir=../data/celebA/ --output_dir=CELEBA_RSLTS_DFR --ckpt_path=CELEBA_RSLTS_TC_2024-04-05_195615/final_checkpoint.pt --tune_class_weights_dfr_train</t>
+  </si>
+  <si>
+    <t>Args for CELEBA_RSLTS_TC_2024-04-05_195615: C:\deep_learning_project\DPBIA_deep_feature_reweighting\train_classifier.py --output_dir=CELEBA_RSLTS_TC --pretrained_model --num_epochs=39 --weight_decay=1e-4 --batch_size=64 --init_lr=1e-3 --eval_freq=1 --data_dir=../data/celebA/ --test_wb_dir=../data/celebA/ --augment_data --seed=16 --resume=CELEBA_RSLTS_TC_2024-04-05_151451/tmp_checkpoint.pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\deep_learning_project\DPBIA_deep_feature_reweighting\venv\Scripts\python.exe C:\deep_learning_project\DPBIA_deep_feature_reweighting\dfr_unpickle.py --pkl_path=CELEBA_RSLTS_DFR_2024-04-06_131241/results.pkl </t>
+  </si>
+  <si>
+    <t>{'base_model_results': {'test': {'accuracy_0_0': 0.9600696221971946,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 'accuracy_0_1': 0.993364299933643,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 'accuracy_1_0': 0.8407258064516129,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 'accuracy_1_1': 0.42777777777777776,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 'mean_accuracy': 0.9530107203687005,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 'worst_accuracy': 0.42777777777777776},</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                        'train': {'accuracy_0_0': 0.99909254631504,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  'accuracy_0_1': 0.9997756975805245,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  'accuracy_1_0': 0.9974650349650349,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  'accuracy_1_1': 0.9920692141312184,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  'mean_accuracy': 0.9990845978988757,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  'worst_accuracy': 0.9920692141312184},</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                        'val': {'accuracy_0_0': 0.9516110134739308,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                'accuracy_0_1': 0.9942000966650556,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                'accuracy_1_0': 0.8583855254001391,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                'accuracy_1_1': 0.37362637362637363,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                'mean_accuracy': 0.9505712991392762,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                'worst_accuracy': 0.37362637362637363}},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dfr_train_results': {'best_hypers': (0.3, 1, 1000.0),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_accs': [0.8659772704003277,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.9385534173855342,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.9649193548387097,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.8055555555555556],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_mean_acc': 0.9051197274822163,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_worst_acc': 0.8055555555555556,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'train_accs': [0.9206921413121846,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                      0.9762076423936553,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                      1.0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                      1.0]},</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_accs': [0.9053957202825842,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.911877903118779,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.9407258064516129,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.8833333333333333],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_mean_acc': 0.9120328624386334,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_worst_acc': 0.8833333333333333,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'train_accs': [0.9230769230769231,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    0.9175824175824175,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    0.989010989010989,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\deep_learning_project\DPBIA_deep_feature_reweighting\venv\Scripts\python.exe C:\deep_learning_project\DPBIA_deep_feature_reweighting\dfr_unpickle.py --pkl_path=CELEBA_RSLTS_DFR_2024-04-06_134259/results.pkl </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dfr_train_results': {'best_hypers': (0.3, 1, 300.0),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_accs': [0.8754991297225351,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.9463835434638355,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.9612903225806452,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.7777777777777778],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_mean_acc': 0.9120328624386334,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_worst_acc': 0.7777777777777778,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'train_accs': [0.9271809661139149,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                      0.969718817591925,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_accs': [0.9013002969181939,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.9185136031851361,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.944758064516129,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.8666666666666667],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_mean_acc': 0.9128844805129747,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_worst_acc': 0.8666666666666667,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'train_accs': [0.8791208791208791,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    0.9285714285714286,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    0.9615384615384616,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    0.9945054945054945]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\deep_learning_project\DPBIA_deep_feature_reweighting\venv\Scripts\python.exe C:\deep_learning_project\DPBIA_deep_feature_reweighting\dfr_unpickle.py --pkl_path=CELEBA_RSLTS_DFR_2024-04-06_141040/results.pkl </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dfr_train_results': {'best_hypers': (0.07, 1, 300.0),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_accs': [0.8576840380874373,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.9348374253483742,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.9705645161290323,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.8111111111111111],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_mean_acc': 0.9004107804829176,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_worst_acc': 0.8111111111111111,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'train_accs': [0.8990627253064167,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                      0.9488103821196827,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_accs': [0.8997645131565476,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.9147976111479761,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.8777777777777778],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_mean_acc': 0.910830578098387,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_worst_acc': 0.8777777777777778,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    0.9560439560439561,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\deep_learning_project\DPBIA_deep_feature_reweighting\venv\Scripts\python.exe C:\deep_learning_project\DPBIA_deep_feature_reweighting\dfr_unpickle.py --pkl_path=CELEBA_RSLTS_DFR_2024-04-06_145554/results.pkl </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dfr_train_results': {'best_hypers': (0.01, 1, 10.0),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_accs': [0.8696631514282789,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.9390842733908428,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.9689516129032258,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.7888888888888889],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_mean_acc': 0.9074742009818656,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_worst_acc': 0.7888888888888889,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'train_accs': [0.9199711607786589,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                      0.9545782263878875,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dfr_val_results': {'best_hypers': (0.7, 1.0, 1.0),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_accs': [0.8982287293949012,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.9124087591240876,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.9495967741935484,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.8888888888888888],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_mean_acc': 0.9098787696623585,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_worst_acc': 0.8888888888888888,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'train_accs': [0.8901098901098901,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    0.9120879120879121,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    0.9505494505494505,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\deep_learning_project\DPBIA_deep_feature_reweighting\venv\Scripts\python.exe C:\deep_learning_project\DPBIA_deep_feature_reweighting\dfr_unpickle.py --pkl_path=CELEBA_RSLTS_DFR_2024-04-06_153458/results.pkl </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'dfr_train_results': {'best_hypers': (0.7, 1, 1000.0),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_accs': [0.8699703081806082,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.9406768414067684,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     0.9637096774193549,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'test_mean_acc': 0.9075743913435528,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       'train_accs': [0.9257390050468637,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                      0.9675558759913482,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_accs': [0.9001740554929866,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.9125414731254148,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   0.9451612903225807,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     'test_mean_acc': 0.9102795311091073,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    0.967032967032967,</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.00000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="182" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1091,6 +1466,23 @@
       <color rgb="FF0C0D0E"/>
       <name val="Var(--ff-mono)"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1124,7 +1516,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1151,14 +1543,26 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="182" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1177,6 +1581,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Damian Smith (ds5n23)" id="{A3DD9A6C-7257-4968-8725-A957E2442D0A}" userId="S::ds5n23@soton.ac.uk::1909826c-daf2-4b03-b6f9-434a2c49888b" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1474,12 +1884,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B27" dT="2024-04-06T12:01:44.93" personId="{A3DD9A6C-7257-4968-8725-A957E2442D0A}" id="{1049BCA2-D16F-4A49-86F1-791FBB17D5A7}">
+    <text>Interupted run - ran epochs 0-11 then 0-38 (which is 51 rather than intended 50)</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BF2C77-194D-4C74-8EF8-245AE7739130}">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A34" sqref="A34:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2118,8 +2536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314D6D9F-A821-4BF3-BE4D-B65BBE98B4B6}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H43" sqref="H43:I45"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3324,14 +3742,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915E905E-2A03-4723-878F-B49E2B2557DF}">
-  <dimension ref="A1:A22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915E905E-2A03-4723-878F-B49E2B2557DF}">
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -3413,37 +3834,1333 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>206</v>
       </c>
     </row>
+    <row r="25" spans="1:2">
+      <c r="B25" s="13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="8" t="str">
+        <f>RIGHT(B25,LEN(B25)-FIND("seed=",B25)-4)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="B33" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B35" s="10">
+        <f>_xlfn.NUMBERVALUE(MID(B31,LEN(B31)-56,17))</f>
+        <v>0.95301072036870005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" s="10">
+        <f>_xlfn.NUMBERVALUE(MID(B31,LEN(B31)-19,19))</f>
+        <v>0.42777777777777698</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B37" s="10"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B38" s="10">
+        <f>_xlfn.NUMBERVALUE(MID(B33,LEN(B33)-56,17))</f>
+        <v>0.95057129913927596</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="10">
+        <f>_xlfn.NUMBERVALUE(MID(B33,LEN(B33)-19,18))</f>
+        <v>0.37362637362637302</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348D72D0-1770-4DD8-B34D-D7EE2E46359A}">
+  <dimension ref="A1:L51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47:H51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="45.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" s="3" customFormat="1">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" s="1" customFormat="1">
+      <c r="B31" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" s="3" customFormat="1">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="1"/>
+      <c r="B47" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(B28,19),18))</f>
+        <v>0.90511972748221603</v>
+      </c>
+      <c r="C47" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(C28,19),18))</f>
+        <v>0.91203286243863302</v>
+      </c>
+      <c r="D47" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(D28,19),18))</f>
+        <v>0.90041078048291701</v>
+      </c>
+      <c r="E47" s="15">
+        <f t="shared" ref="E47:F47" si="0">_xlfn.NUMBERVALUE(LEFT(RIGHT(E28,19),18))</f>
+        <v>0.90747420098186504</v>
+      </c>
+      <c r="F47" s="15">
+        <f t="shared" si="0"/>
+        <v>0.907574391343552</v>
+      </c>
+      <c r="G47" s="16">
+        <f t="shared" ref="G47:G48" si="1">AVERAGE(B47:F47)</f>
+        <v>0.90652239254583655</v>
+      </c>
+      <c r="H47" s="16">
+        <f>_xlfn.STDEV.S(B47:F47)</f>
+        <v>4.2337096764253727E-3</v>
+      </c>
+      <c r="I47" t="s">
+        <v>143</v>
+      </c>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="1"/>
+      <c r="B48" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(B29,19),18))</f>
+        <v>0.80555555555555503</v>
+      </c>
+      <c r="C48" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(C29,19),18))</f>
+        <v>0.77777777777777701</v>
+      </c>
+      <c r="D48" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(D29,19),18))</f>
+        <v>0.81111111111111101</v>
+      </c>
+      <c r="E48" s="15">
+        <f t="shared" ref="E48:F48" si="2">_xlfn.NUMBERVALUE(LEFT(RIGHT(E29,19),18))</f>
+        <v>0.78888888888888797</v>
+      </c>
+      <c r="F48" s="15">
+        <f t="shared" si="2"/>
+        <v>0.78888888888888797</v>
+      </c>
+      <c r="G48" s="16">
+        <f t="shared" si="1"/>
+        <v>0.79444444444444373</v>
+      </c>
+      <c r="H48" s="16">
+        <f t="shared" ref="H48:H51" si="3">_xlfn.STDEV.S(B48:F48)</f>
+        <v>1.3608276348795714E-2</v>
+      </c>
+      <c r="I48" t="s">
+        <v>145</v>
+      </c>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="2:9">
+      <c r="B49" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+    </row>
+    <row r="50" spans="2:9">
+      <c r="B50" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(B39,19),18))</f>
+        <v>0.91203286243863302</v>
+      </c>
+      <c r="C50" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(C39,19),18))</f>
+        <v>0.91288448051297399</v>
+      </c>
+      <c r="D50" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(D39,19),18))</f>
+        <v>0.91083057809838697</v>
+      </c>
+      <c r="E50" s="15">
+        <f t="shared" ref="E50:F50" si="4">_xlfn.NUMBERVALUE(LEFT(RIGHT(E39,19),18))</f>
+        <v>0.90987876966235803</v>
+      </c>
+      <c r="F50" s="15">
+        <f t="shared" si="4"/>
+        <v>0.91027953110910698</v>
+      </c>
+      <c r="G50" s="16">
+        <f>AVERAGE(B50:F50)</f>
+        <v>0.91118124436429182</v>
+      </c>
+      <c r="H50" s="16">
+        <f t="shared" si="3"/>
+        <v>1.2508757628677102E-3</v>
+      </c>
+      <c r="I50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9">
+      <c r="B51" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(B40,19),18))</f>
+        <v>0.88333333333333297</v>
+      </c>
+      <c r="C51" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(C40,19),18))</f>
+        <v>0.86666666666666603</v>
+      </c>
+      <c r="D51" s="15">
+        <f>_xlfn.NUMBERVALUE(LEFT(RIGHT(D40,19),18))</f>
+        <v>0.87777777777777699</v>
+      </c>
+      <c r="E51" s="15">
+        <f t="shared" ref="E51:F51" si="5">_xlfn.NUMBERVALUE(LEFT(RIGHT(E40,19),18))</f>
+        <v>0.88888888888888795</v>
+      </c>
+      <c r="F51" s="15">
+        <f t="shared" si="5"/>
+        <v>0.88333333333333297</v>
+      </c>
+      <c r="G51" s="16">
+        <f>AVERAGE(B51:F51)</f>
+        <v>0.87999999999999934</v>
+      </c>
+      <c r="H51" s="16">
+        <f t="shared" si="3"/>
+        <v>8.4254171600572636E-3</v>
+      </c>
+      <c r="I51" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>